<commit_message>
update dvdd, thich nghi
</commit_message>
<xml_diff>
--- a/Landuse_MK_GEMMES/includes/codeloaidat.xlsx
+++ b/Landuse_MK_GEMMES/includes/codeloaidat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcquang\Downloads\ht2050_mkd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_mohinhGEMMES\WP4_SocTrang\Landuse_MK_GEMMES\includes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>BHK</t>
   </si>
@@ -69,19 +69,69 @@
   </si>
   <si>
     <t>1 vu</t>
+  </si>
+  <si>
+    <t>LUT2</t>
+  </si>
+  <si>
+    <t>2lua</t>
+  </si>
+  <si>
+    <t>LUT3</t>
+  </si>
+  <si>
+    <t>lua-mau</t>
+  </si>
+  <si>
+    <t>LUT4</t>
+  </si>
+  <si>
+    <t>lua-tom</t>
+  </si>
+  <si>
+    <t>LUT5</t>
+  </si>
+  <si>
+    <t>khom-mia</t>
+  </si>
+  <si>
+    <t>LUT6</t>
+  </si>
+  <si>
+    <t>mau</t>
+  </si>
+  <si>
+    <t>LUT7</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>LUT8</t>
+  </si>
+  <si>
+    <t>thuysanman</t>
+  </si>
+  <si>
+    <t>lua 1 vu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,8 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D13"/>
+  <dimension ref="B1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -405,7 +459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -415,8 +469,17 @@
       <c r="D2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -426,8 +489,17 @@
       <c r="D3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -437,8 +509,17 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -448,8 +529,17 @@
       <c r="D5">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -459,8 +549,17 @@
       <c r="D6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -470,8 +569,17 @@
       <c r="D7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -481,8 +589,17 @@
       <c r="D8">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>9</v>
       </c>
@@ -492,8 +609,12 @@
       <c r="D9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>10</v>
       </c>
@@ -504,7 +625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>11</v>
       </c>
@@ -515,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>12</v>
       </c>
@@ -526,7 +647,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>8</v>
       </c>
@@ -536,6 +657,29 @@
       <c r="D13">
         <v>0</v>
       </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>104</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2">
+        <v>105</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>